<commit_message>
Modification de la liste des tests
</commit_message>
<xml_diff>
--- a/Liste_des_tests.xlsx
+++ b/Liste_des_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
   <si>
     <t>Trombinoscope</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Autres</t>
+  </si>
+  <si>
+    <t>bug détecté : "la date de fin est antérieure" -&gt; faux, elle est égale (juste modifier texte affiché) + au lieu de concaténer les deux nombres, les convertir directement en dates</t>
   </si>
 </sst>
 </file>
@@ -298,8 +301,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D10"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,12 +631,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -677,12 +680,12 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -695,12 +698,12 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -760,12 +763,12 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -817,12 +820,12 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
@@ -879,7 +882,7 @@
         <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,100 +924,100 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>63</v>
-      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>70</v>
-      </c>
-      <c r="C57" t="s">
-        <v>71</v>
-      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="C58" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>73</v>
-      </c>
-      <c r="C59" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C60" t="s">
         <v>71</v>
       </c>
     </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A57:D57"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A48:D48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modification fichier suivi de tests + correction bug profil alertes stagiaire
</commit_message>
<xml_diff>
--- a/Liste_des_tests.xlsx
+++ b/Liste_des_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="81">
   <si>
     <t>Trombinoscope</t>
   </si>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>bug détecté : "la date de fin est antérieure" -&gt; faux, elle est égale (juste modifier texte affiché) + au lieu de concaténer les deux nombres, les convertir directement en dates</t>
+  </si>
+  <si>
+    <t>Afficher le trombinoscpe d'une liste de stagiaire ne possédant pas de photos</t>
+  </si>
+  <si>
+    <t>bug détecté : revoir la gestion de l'url, elles semblent classées dans un dossier.</t>
+  </si>
+  <si>
+    <t>Soumission d'une absence temporaire sans saisir de nom</t>
+  </si>
+  <si>
+    <t>bug détecté : pas d'avertissement. -&gt; mettre un messagebox.show pour dire  qu'il n'y a pas de stagiaire sélectionné.</t>
   </si>
 </sst>
 </file>
@@ -604,16 +616,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="90" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="157.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -660,342 +672,348 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
+      <c r="A25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" t="s">
-        <v>46</v>
-      </c>
+      <c r="A34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="C37" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="C41" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>56</v>
+        <v>47</v>
+      </c>
+      <c r="C42" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>58</v>
-      </c>
-      <c r="C44" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C45" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>64</v>
-      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+      <c r="B57" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>70</v>
-      </c>
-      <c r="C58" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>72</v>
-      </c>
+      <c r="A59" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C60" t="s">
         <v>71</v>
@@ -1003,21 +1021,34 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>74</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C63" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A59:D59"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A50:D50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correction de nombreux bugs
</commit_message>
<xml_diff>
--- a/Liste_des_tests.xlsx
+++ b/Liste_des_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
   <si>
     <t>Trombinoscope</t>
   </si>
@@ -259,6 +259,18 @@
   </si>
   <si>
     <t>bug détecté : pas d'avertissement. -&gt; mettre un messagebox.show pour dire  qu'il n'y a pas de stagiaire sélectionné.</t>
+  </si>
+  <si>
+    <t>bug détecté : après ajout, l'item sélectionné n'est pas le dernier de la liste</t>
+  </si>
+  <si>
+    <t>Supppression d'une observation</t>
+  </si>
+  <si>
+    <t>Suppression d'une observation sans sélection</t>
+  </si>
+  <si>
+    <t>amélioration possible : modifier le format de la colonne durée pour que ce soit human readable</t>
   </si>
 </sst>
 </file>
@@ -616,15 +628,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.42578125" customWidth="1"/>
     <col min="3" max="3" width="157.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -782,6 +794,9 @@
       <c r="C22" t="s">
         <v>29</v>
       </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -813,11 +828,20 @@
       <c r="C27" t="s">
         <v>34</v>
       </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>33</v>
       </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -831,6 +855,9 @@
       <c r="C30" t="s">
         <v>36</v>
       </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -844,189 +871,219 @@
       <c r="C32" t="s">
         <v>39</v>
       </c>
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" t="s">
-        <v>46</v>
-      </c>
+      <c r="A36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>52</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>56</v>
+        <v>47</v>
+      </c>
+      <c r="C44" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>58</v>
-      </c>
-      <c r="C46" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s">
-        <v>60</v>
+        <v>52</v>
+      </c>
+      <c r="D47" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>64</v>
-      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+      <c r="B59" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>72</v>
-      </c>
+      <c r="A61" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C62" t="s">
         <v>71</v>
@@ -1034,21 +1091,34 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>74</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C65" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A61:D61"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A52:D52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update rapide sur liste des tests avant de manger :-)
</commit_message>
<xml_diff>
--- a/Liste_des_tests.xlsx
+++ b/Liste_des_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
   <si>
     <t>Trombinoscope</t>
   </si>
@@ -252,9 +252,6 @@
     <t>Afficher le trombinoscpe d'une liste de stagiaire ne possédant pas de photos</t>
   </si>
   <si>
-    <t>bug détecté : revoir la gestion de l'url, elles semblent classées dans un dossier.</t>
-  </si>
-  <si>
     <t>Soumission d'une absence temporaire sans saisir de nom</t>
   </si>
   <si>
@@ -271,6 +268,21 @@
   </si>
   <si>
     <t>amélioration possible : modifier le format de la colonne durée pour que ce soit human readable</t>
+  </si>
+  <si>
+    <t>Bandeau recherche stagiaire</t>
+  </si>
+  <si>
+    <t>chargement d'un stagiaire, visualisation d'un form, chargement d'un nouveau stagiaire</t>
+  </si>
+  <si>
+    <t>bug détecté : le form en visualisation ne s'actualise pas avec les infos du stagiaire. (par exemple profil alertes stagiaire)</t>
+  </si>
+  <si>
+    <t>bug détecté : revoir la gestion de l'url, elles semblent classées dans un dossier (envoyer mail à jérome)</t>
+  </si>
+  <si>
+    <t>en attente</t>
   </si>
 </sst>
 </file>
@@ -628,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +699,10 @@
         <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>87</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -726,10 +741,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
         <v>79</v>
-      </c>
-      <c r="C13" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -837,7 +852,7 @@
         <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D28" t="s">
         <v>13</v>
@@ -877,12 +892,12 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -936,7 +951,7 @@
         <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1075,7 +1090,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1083,20 +1098,23 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C62" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>72</v>
-      </c>
+      <c r="A63" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C64" t="s">
         <v>71</v>
@@ -1104,21 +1122,35 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>73</v>
+      </c>
+      <c r="C66" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>74</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C67" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A61:D61"/>
+  <mergeCells count="8">
+    <mergeCell ref="A63:D63"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A61:D61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modification constantes, update du fichier de suivi de tests
</commit_message>
<xml_diff>
--- a/Liste_des_tests.xlsx
+++ b/Liste_des_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
   <si>
     <t>Trombinoscope</t>
   </si>
@@ -283,6 +283,21 @@
   </si>
   <si>
     <t>bug détecté : revoir la gestion de l'url, elles semblent classées dans un dossier (attente réponse mail jérome)</t>
+  </si>
+  <si>
+    <t>Affichage d'un stagiaire n'ayant pas de contact en entreprise</t>
+  </si>
+  <si>
+    <t>Affichage d'un stagiaire ayant plusieurs contacts en entreprise</t>
+  </si>
+  <si>
+    <t>bug détecté : on ne peut pas ajouter ni modifier de contact - idem pour les entreprises… -&gt; un bouton modifier qui renvoie vers une popup ou on peut add/update/delete les contacts</t>
+  </si>
+  <si>
+    <t>En cours</t>
+  </si>
+  <si>
+    <t>Abandonné</t>
   </si>
 </sst>
 </file>
@@ -332,18 +347,127 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -640,16 +764,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="73.42578125" customWidth="1"/>
     <col min="3" max="3" width="157.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -662,7 +787,7 @@
       <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -701,7 +826,7 @@
       <c r="C7" t="s">
         <v>88</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
         <v>87</v>
       </c>
     </row>
@@ -722,7 +847,7 @@
       <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -772,7 +897,7 @@
       <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -783,7 +908,7 @@
       <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -809,7 +934,7 @@
       <c r="C22" t="s">
         <v>29</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -822,291 +947,294 @@
       <c r="B24" t="s">
         <v>27</v>
       </c>
+      <c r="D24" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" t="s">
-        <v>13</v>
-      </c>
+      <c r="A27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>82</v>
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" t="s">
-        <v>13</v>
-      </c>
+      <c r="A38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>48</v>
-      </c>
-      <c r="D39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>46</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="C41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" t="s">
-        <v>54</v>
-      </c>
-      <c r="D43" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="C45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>56</v>
+        <v>47</v>
+      </c>
+      <c r="C46" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" t="s">
-        <v>52</v>
-      </c>
-      <c r="D47" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>58</v>
-      </c>
-      <c r="C48" t="s">
-        <v>54</v>
-      </c>
-      <c r="D48" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" t="s">
+        <v>60</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>64</v>
-      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="B61" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>85</v>
-      </c>
-      <c r="C62" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -1114,46 +1242,119 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>70</v>
-      </c>
-      <c r="C64" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>73</v>
       </c>
       <c r="C66" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>74</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C69" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A65:D65"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A63:D63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{833CDF47-4986-4238-BA11-5C7A7E953575}">
+            <xm:f>NOT(ISERROR(SEARCH($D$17,D1)))</xm:f>
+            <xm:f>$D$17</xm:f>
+            <x14:dxf>
+              <numFmt numFmtId="30" formatCode="@"/>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{EB4DE3BD-48BB-4814-BCAF-329AE2D0EB03}">
+            <xm:f>NOT(ISERROR(SEARCH($D$7,D1)))</xm:f>
+            <xm:f>$D$7</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFF00"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{B5B0C31F-17D5-4619-9B88-488C83CA8B05}">
+            <xm:f>NOT(ISERROR(SEARCH($D$24,D1)))</xm:f>
+            <xm:f>$D$24</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{DEFDB3A8-D10D-4562-A517-70E3B906113D}">
+            <xm:f>NOT(ISERROR(SEARCH($D$25,D1)))</xm:f>
+            <xm:f>$D$25</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Début de modifications sur les contacts.
</commit_message>
<xml_diff>
--- a/Liste_des_tests.xlsx
+++ b/Liste_des_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="95">
   <si>
     <t>Trombinoscope</t>
   </si>
@@ -291,13 +291,16 @@
     <t>Affichage d'un stagiaire ayant plusieurs contacts en entreprise</t>
   </si>
   <si>
-    <t>bug détecté : on ne peut pas ajouter ni modifier de contact - idem pour les entreprises… -&gt; un bouton modifier qui renvoie vers une popup ou on peut add/update/delete les contacts</t>
-  </si>
-  <si>
     <t>En cours</t>
   </si>
   <si>
     <t>Abandonné</t>
+  </si>
+  <si>
+    <t>bug détecté : le contact et le stagiaire sont liés bizarrement, ça semble pas tenir la route</t>
+  </si>
+  <si>
+    <t>bug détecté : on ne peut pas ajouter ni modifier de contact - idem pour les entreprises… -&gt; pour les modifs et la suppression : dans datagrid.Pour l'ajout : un boutonqui renvoie vers une popup ou on peut add un contact. Penser à faire des contrôles de saisie (numéros de téléphone par exemple), et vérifier que quand on appuye sur Suppr pour supprimer un caractère, il n'y a pas de demande de supprimer toute la ligne</t>
   </si>
 </sst>
 </file>
@@ -347,24 +350,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -388,79 +394,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
@@ -766,15 +699,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="73.42578125" customWidth="1"/>
     <col min="3" max="3" width="157.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -787,17 +720,17 @@
       <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -826,7 +759,7 @@
       <c r="C7" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>87</v>
       </c>
     </row>
@@ -847,17 +780,17 @@
       <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -871,6 +804,9 @@
       <c r="C13" t="s">
         <v>79</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -878,17 +814,23 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>18</v>
       </c>
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -897,7 +839,7 @@
       <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -908,7 +850,7 @@
       <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -934,7 +876,7 @@
       <c r="C22" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -947,19 +889,19 @@
       <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>89</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -968,12 +910,12 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
@@ -987,7 +929,7 @@
       <c r="C29" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -998,7 +940,7 @@
       <c r="C30" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1014,7 +956,7 @@
       <c r="C32" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1030,7 +972,7 @@
       <c r="C34" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1050,12 +992,12 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
@@ -1064,7 +1006,7 @@
       <c r="C39" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1075,7 +1017,7 @@
       <c r="C40" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1086,7 +1028,7 @@
       <c r="C41" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1110,7 +1052,7 @@
       <c r="C44" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1121,7 +1063,7 @@
       <c r="C45" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1132,7 +1074,7 @@
       <c r="C46" t="s">
         <v>76</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1153,7 +1095,7 @@
       <c r="C49" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1164,7 +1106,7 @@
       <c r="C50" t="s">
         <v>54</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1175,7 +1117,7 @@
       <c r="C51" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1185,12 +1127,12 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
@@ -1233,12 +1175,12 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
@@ -1247,17 +1189,17 @@
       <c r="C64" t="s">
         <v>86</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>92</v>
+      <c r="D64" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">

</xml_diff>

<commit_message>
Avancée sur l'ajout de contacts
</commit_message>
<xml_diff>
--- a/Liste_des_tests.xlsx
+++ b/Liste_des_tests.xlsx
@@ -300,7 +300,8 @@
     <t>bug détecté : le contact et le stagiaire sont liés bizarrement, ça semble pas tenir la route</t>
   </si>
   <si>
-    <t>bug détecté : on ne peut pas ajouter ni modifier de contact - idem pour les entreprises… -&gt; pour les modifs et la suppression : dans datagrid.Pour l'ajout : un boutonqui renvoie vers une popup ou on peut add un contact. Penser à faire des contrôles de saisie (numéros de téléphone par exemple), et vérifier que quand on appuye sur Suppr pour supprimer un caractère, il n'y a pas de demande de supprimer toute la ligne</t>
+    <t>bug détecté : on ne peut pas ajouter ni modifier de contact - idem pour les entreprises… -&gt; pour les modifs et la suppression : dans datagrid.Pour l'ajout : un boutonqui renvoie vers une popup ou on peut add un contact. Penser à faire des contrôles de saisie (numéros de téléphone par exemple), et vérifier que quand on appuye sur Suppr pour supprimer un caractère, il n'y a pas de demande de supprimer toute la ligne
+bug détecté : Même quand la requête ne réussit pas, la popup affiche "suppression effectuée". La requête ne fonctionne pas à cause d'une FK sur la table évenement.Mettre un code retour sur toutes les requêtes.</t>
   </si>
 </sst>
 </file>
@@ -361,11 +362,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,7 +701,7 @@
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,12 +726,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -785,12 +786,12 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -814,12 +815,12 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -893,11 +894,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -910,12 +911,12 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
@@ -992,12 +993,12 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
@@ -1127,12 +1128,12 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
@@ -1175,12 +1176,12 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
@@ -1194,12 +1195,12 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">

</xml_diff>

<commit_message>
Multiples corrections sur les contacts et autres + mise à jour liste des tests
</commit_message>
<xml_diff>
--- a/Liste_des_tests.xlsx
+++ b/Liste_des_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="97">
   <si>
     <t>Trombinoscope</t>
   </si>
@@ -294,14 +294,20 @@
     <t>En cours</t>
   </si>
   <si>
-    <t>Abandonné</t>
-  </si>
-  <si>
-    <t>bug détecté : le contact et le stagiaire sont liés bizarrement, ça semble pas tenir la route</t>
-  </si>
-  <si>
-    <t>bug détecté : on ne peut pas ajouter ni modifier de contact - idem pour les entreprises… -&gt; pour les modifs et la suppression : dans datagrid.Pour l'ajout : un boutonqui renvoie vers une popup ou on peut add un contact. Penser à faire des contrôles de saisie (numéros de téléphone par exemple), et vérifier que quand on appuye sur Suppr pour supprimer un caractère, il n'y a pas de demande de supprimer toute la ligne
-bug détecté : Même quand la requête ne réussit pas, la popup affiche "suppression effectuée". La requête ne fonctionne pas à cause d'une FK sur la table évenement.Mettre un code retour sur toutes les requêtes.</t>
+    <t xml:space="preserve">bug détecté : on ne peut pas ajouter ni modifier de contact - idem pour les entreprises… 
+bug détecté : Même quand la requête ne réussit pas, la popup affiche "suppression effectuée". </t>
+  </si>
+  <si>
+    <t>incohérence : le formulaire est nommé "absence rapide", et lorsqu'une absence est ajoutée, "Retard ajouté" est affiché. (+ faute de frappe)</t>
+  </si>
+  <si>
+    <t>A compléter avec les opérations sur les contacts, les entreprises…..</t>
+  </si>
+  <si>
+    <t>bug détecté : Lors de la modification d'un contact, on peut lui enlever ses 2 numéros de téléphone</t>
+  </si>
+  <si>
+    <t>bug détecté : le contact et le stagiaire sont liés bizarrement, ça ne tient pas trop la route. La correction apporte une gestion plus souple.</t>
   </si>
 </sst>
 </file>
@@ -371,7 +377,94 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="16">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -698,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,6 +890,12 @@
       <c r="B12" t="s">
         <v>15</v>
       </c>
+      <c r="C12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -827,7 +926,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>13</v>
@@ -890,19 +989,16 @@
       <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>89</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -911,35 +1007,35 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>31</v>
-      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>13</v>
@@ -947,76 +1043,76 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="C31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>81</v>
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>13</v>
@@ -1024,10 +1120,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>13</v>
@@ -1035,34 +1131,34 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>48</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="C43" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" t="s">
-        <v>52</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>13</v>
@@ -1070,10 +1166,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>13</v>
@@ -1081,31 +1177,31 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>55</v>
+        <v>47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" t="s">
-        <v>52</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>13</v>
@@ -1113,10 +1209,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>13</v>
@@ -1124,180 +1220,165 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>63</v>
-      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>85</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>86</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>70</v>
-      </c>
-      <c r="C66" t="s">
-        <v>71</v>
-      </c>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="C67" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>73</v>
-      </c>
-      <c r="C68" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C69" t="s">
         <v>71</v>
       </c>
     </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A66:D66"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A64:D64"/>
   </mergeCells>
+  <conditionalFormatting sqref="D1:D26 D28:D1048576">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Abandonné">
+      <formula>NOT(ISERROR(SEARCH("Abandonné",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="en attente">
+      <formula>NOT(ISERROR(SEARCH("en attente",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Corrigé">
+      <formula>NOT(ISERROR(SEARCH("Corrigé",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Abandonné">
+      <formula>NOT(ISERROR(SEARCH("Abandonné",D27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="en attente">
+      <formula>NOT(ISERROR(SEARCH("en attente",D27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Corrigé">
+      <formula>NOT(ISERROR(SEARCH("Corrigé",D27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{833CDF47-4986-4238-BA11-5C7A7E953575}">
-            <xm:f>NOT(ISERROR(SEARCH($D$17,D1)))</xm:f>
-            <xm:f>$D$17</xm:f>
-            <x14:dxf>
-              <numFmt numFmtId="30" formatCode="@"/>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF92D050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{EB4DE3BD-48BB-4814-BCAF-329AE2D0EB03}">
-            <xm:f>NOT(ISERROR(SEARCH($D$7,D1)))</xm:f>
-            <xm:f>$D$7</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFFF00"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{B5B0C31F-17D5-4619-9B88-488C83CA8B05}">
-            <xm:f>NOT(ISERROR(SEARCH($D$24,D1)))</xm:f>
-            <xm:f>$D$24</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFF0000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{DEFDB3A8-D10D-4562-A517-70E3B906113D}">
-            <xm:f>NOT(ISERROR(SEARCH($D$25,D1)))</xm:f>
-            <xm:f>$D$25</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>D1:D1048576</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
2-3 modifs sur les contacts.
</commit_message>
<xml_diff>
--- a/Liste_des_tests.xlsx
+++ b/Liste_des_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="112">
   <si>
     <t>Trombinoscope</t>
   </si>
@@ -294,20 +294,65 @@
     <t>En cours</t>
   </si>
   <si>
-    <t xml:space="preserve">bug détecté : on ne peut pas ajouter ni modifier de contact - idem pour les entreprises… 
+    <t>incohérence : le formulaire est nommé "absence rapide", et lorsqu'une absence est ajoutée, "Retard ajouté" est affiché. (+ faute de frappe)</t>
+  </si>
+  <si>
+    <t>A compléter avec les opérations sur les contacts, les entreprises…..</t>
+  </si>
+  <si>
+    <t>bug détecté : Lors de la modification d'un contact, on peut lui enlever ses 2 numéros de téléphone</t>
+  </si>
+  <si>
+    <t>bug détecté : le contact et le stagiaire sont liés bizarrement, ça ne tient pas trop la route. La correction apporte une gestion plus souple.</t>
+  </si>
+  <si>
+    <t>Ajout d'un contact provenant d'une entreprise existante</t>
+  </si>
+  <si>
+    <t>Ajout d'un contact avec ajout d'une nouvelle entreprise</t>
+  </si>
+  <si>
+    <t>Ajout d'un contact sans entreprise</t>
+  </si>
+  <si>
+    <t>Ajout d'un contact sans fonction</t>
+  </si>
+  <si>
+    <t>Ajout d'un contact sans numéro de téléphone fixe ni portable</t>
+  </si>
+  <si>
+    <t>Ajout d'un contact sans nom</t>
+  </si>
+  <si>
+    <t>Ajout d'une entreprise sans raison sociale</t>
+  </si>
+  <si>
+    <t>Ajout d'une entreprise</t>
+  </si>
+  <si>
+    <t>Modification d'un contact</t>
+  </si>
+  <si>
+    <t>Modification d'un contact en supprimant ses deux numéros de téléphone</t>
+  </si>
+  <si>
+    <t>Tentative de modification de l'entreprise d'un contact</t>
+  </si>
+  <si>
+    <t>Tentative de modification de la fonction du contact</t>
+  </si>
+  <si>
+    <t>Ajout d'un contact sans aucun champs positionné</t>
+  </si>
+  <si>
+    <t>Suppression d'un contact</t>
+  </si>
+  <si>
+    <t>Suppression d'un contact ayant des enregistrements dans la table observations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Améliration : modifier un contact
 bug détecté : Même quand la requête ne réussit pas, la popup affiche "suppression effectuée". </t>
-  </si>
-  <si>
-    <t>incohérence : le formulaire est nommé "absence rapide", et lorsqu'une absence est ajoutée, "Retard ajouté" est affiché. (+ faute de frappe)</t>
-  </si>
-  <si>
-    <t>A compléter avec les opérations sur les contacts, les entreprises…..</t>
-  </si>
-  <si>
-    <t>bug détecté : Lors de la modification d'un contact, on peut lui enlever ses 2 numéros de téléphone</t>
-  </si>
-  <si>
-    <t>bug détecté : le contact et le stagiaire sont liés bizarrement, ça ne tient pas trop la route. La correction apporte une gestion plus souple.</t>
   </si>
 </sst>
 </file>
@@ -377,7 +422,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="64">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -466,6 +511,21 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
@@ -480,6 +540,14 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -487,10 +555,335 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -791,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,7 +1284,7 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>13</v>
@@ -926,13 +1319,13 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>19</v>
       </c>
@@ -943,7 +1336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>21</v>
       </c>
@@ -954,22 +1347,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>26</v>
       </c>
@@ -980,196 +1373,137 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>89</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" t="s">
         <v>94</v>
       </c>
-      <c r="C27" t="s">
-        <v>95</v>
-      </c>
       <c r="D27" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>50</v>
-      </c>
+      <c r="A44" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C46" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>13</v>
@@ -1177,10 +1511,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C47" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>13</v>
@@ -1188,31 +1522,31 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>56</v>
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>57</v>
-      </c>
-      <c r="C50" t="s">
-        <v>52</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>13</v>
@@ -1220,23 +1554,22 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>61</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -1244,137 +1577,342 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>63</v>
+        <v>43</v>
+      </c>
+      <c r="C56" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>64</v>
+        <v>45</v>
+      </c>
+      <c r="C57" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>41</v>
+        <v>47</v>
+      </c>
+      <c r="C58" t="s">
+        <v>48</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>65</v>
+        <v>49</v>
+      </c>
+      <c r="C59" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>67</v>
+        <v>51</v>
+      </c>
+      <c r="C61" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>69</v>
+        <v>53</v>
+      </c>
+      <c r="C62" t="s">
+        <v>54</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>68</v>
+        <v>47</v>
+      </c>
+      <c r="C63" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+      <c r="B64" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>85</v>
-      </c>
-      <c r="C65" t="s">
-        <v>86</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
+      <c r="B66" t="s">
+        <v>57</v>
+      </c>
+      <c r="C66" t="s">
+        <v>52</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C67" t="s">
-        <v>71</v>
+        <v>54</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>72</v>
+        <v>59</v>
+      </c>
+      <c r="C68" t="s">
+        <v>60</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>85</v>
+      </c>
+      <c r="C81" t="s">
+        <v>86</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>70</v>
+      </c>
+      <c r="C83" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
         <v>73</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C85" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>74</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C86" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A82:D82"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A44:D44"/>
     <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A80:D80"/>
   </mergeCells>
-  <conditionalFormatting sqref="D1:D26 D28:D1048576">
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Abandonné">
+  <conditionalFormatting sqref="D1:D26 D44:D1048576">
+    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="Abandonné">
       <formula>NOT(ISERROR(SEARCH("Abandonné",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="en attente">
+    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="en attente">
       <formula>NOT(ISERROR(SEARCH("en attente",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Corrigé">
+    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="Corrigé">
       <formula>NOT(ISERROR(SEARCH("Corrigé",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Abandonné">
+  <conditionalFormatting sqref="D27:D37 D43">
+    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Abandonné">
       <formula>NOT(ISERROR(SEARCH("Abandonné",D27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="en attente">
+    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="en attente">
       <formula>NOT(ISERROR(SEARCH("en attente",D27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Corrigé">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="Corrigé">
       <formula>NOT(ISERROR(SEARCH("Corrigé",D27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="Abandonné">
+      <formula>NOT(ISERROR(SEARCH("Abandonné",D38)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D38)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="en attente">
+      <formula>NOT(ISERROR(SEARCH("en attente",D38)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="Corrigé">
+      <formula>NOT(ISERROR(SEARCH("Corrigé",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Abandonné">
+      <formula>NOT(ISERROR(SEARCH("Abandonné",D42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="en attente">
+      <formula>NOT(ISERROR(SEARCH("en attente",D42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="Corrigé">
+      <formula>NOT(ISERROR(SEARCH("Corrigé",D42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Abandonné">
+      <formula>NOT(ISERROR(SEARCH("Abandonné",D41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="en attente">
+      <formula>NOT(ISERROR(SEARCH("en attente",D41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="Corrigé">
+      <formula>NOT(ISERROR(SEARCH("Corrigé",D41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Abandonné">
+      <formula>NOT(ISERROR(SEARCH("Abandonné",D40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="en attente">
+      <formula>NOT(ISERROR(SEARCH("en attente",D40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Corrigé">
+      <formula>NOT(ISERROR(SEARCH("Corrigé",D40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Abandonné">
+      <formula>NOT(ISERROR(SEARCH("Abandonné",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="en attente">
+      <formula>NOT(ISERROR(SEARCH("en attente",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Corrigé">
+      <formula>NOT(ISERROR(SEARCH("Corrigé",D39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nouveau bug listé dans la liste des tests + mise à jour du manuel d'utilisation + petite correcction sur le format de date au niveau des observations
</commit_message>
<xml_diff>
--- a/Liste_des_tests.xlsx
+++ b/Liste_des_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="117">
   <si>
     <t>Trombinoscope</t>
   </si>
@@ -353,6 +353,21 @@
   <si>
     <t xml:space="preserve">Améliration : modifier un contact
 bug détecté : Même quand la requête ne réussit pas, la popup affiche "suppression effectuée". </t>
+  </si>
+  <si>
+    <t>Clic sur le bouton Annuler</t>
+  </si>
+  <si>
+    <t>Clic sur le bouton Annuler après avoir saisi une nouvelle absence</t>
+  </si>
+  <si>
+    <t>Clic sur le bouton Annuler après avoir modifié une absence existante</t>
+  </si>
+  <si>
+    <t>Consultation d'une observation</t>
+  </si>
+  <si>
+    <t>bug détecté : le format de l'heure dans la date n'est pas bon : l'heure est 00:00:00. Voir fomat de date à l'affichage</t>
   </si>
 </sst>
 </file>
@@ -422,94 +437,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="64">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="52">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -1184,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,10 +1428,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
       <c r="C46" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>13</v>
@@ -1511,10 +1439,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>13</v>
@@ -1522,111 +1450,102 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="C48" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>40</v>
-      </c>
-      <c r="C49" t="s">
-        <v>36</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="C50" t="s">
+        <v>36</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" t="s">
-        <v>39</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>81</v>
+        <v>38</v>
+      </c>
+      <c r="C52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>43</v>
-      </c>
-      <c r="C56" t="s">
-        <v>44</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>45</v>
-      </c>
-      <c r="C57" t="s">
-        <v>46</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>13</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>47</v>
-      </c>
-      <c r="C58" t="s">
-        <v>48</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>49</v>
-      </c>
-      <c r="C59" t="s">
-        <v>83</v>
-      </c>
+      <c r="A59" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="C60" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>13</v>
@@ -1634,10 +1553,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C62" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>13</v>
@@ -1645,31 +1564,34 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C63" t="s">
-        <v>76</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="C65" t="s">
+        <v>52</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C66" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>13</v>
@@ -1677,10 +1599,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C67" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>13</v>
@@ -1688,231 +1610,305 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>59</v>
-      </c>
-      <c r="C68" t="s">
-        <v>60</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>57</v>
+      </c>
+      <c r="C70" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
+      <c r="B71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C71" t="s">
+        <v>54</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="C72" t="s">
+        <v>60</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>65</v>
-      </c>
+      <c r="A75" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
+      <c r="B80" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>85</v>
-      </c>
-      <c r="C81" t="s">
-        <v>86</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
+      <c r="B82" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>70</v>
-      </c>
-      <c r="C83" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>72</v>
-      </c>
+      <c r="A84" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
+        <v>85</v>
+      </c>
+      <c r="C85" t="s">
+        <v>86</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>70</v>
+      </c>
+      <c r="C87" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
         <v>73</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C89" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
         <v>74</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C90" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A86:D86"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A84:D84"/>
   </mergeCells>
-  <conditionalFormatting sqref="D1:D26 D44:D1048576">
-    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="Abandonné">
+  <conditionalFormatting sqref="D1:D26 D44:D54 D59:D1048576 D57">
+    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="Abandonné">
       <formula>NOT(ISERROR(SEARCH("Abandonné",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="38" priority="46" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="en attente">
+    <cfRule type="containsText" dxfId="37" priority="47" operator="containsText" text="en attente">
       <formula>NOT(ISERROR(SEARCH("en attente",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="Corrigé">
+    <cfRule type="containsText" dxfId="36" priority="48" operator="containsText" text="Corrigé">
       <formula>NOT(ISERROR(SEARCH("Corrigé",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D37 D43">
-    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Abandonné">
+    <cfRule type="containsText" dxfId="35" priority="41" operator="containsText" text="Abandonné">
       <formula>NOT(ISERROR(SEARCH("Abandonné",D27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="34" priority="42" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="en attente">
+    <cfRule type="containsText" dxfId="33" priority="43" operator="containsText" text="en attente">
       <formula>NOT(ISERROR(SEARCH("en attente",D27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="Corrigé">
+    <cfRule type="containsText" dxfId="32" priority="44" operator="containsText" text="Corrigé">
       <formula>NOT(ISERROR(SEARCH("Corrigé",D27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="Abandonné">
+    <cfRule type="containsText" dxfId="31" priority="37" operator="containsText" text="Abandonné">
       <formula>NOT(ISERROR(SEARCH("Abandonné",D38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="30" priority="38" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="en attente">
+    <cfRule type="containsText" dxfId="29" priority="39" operator="containsText" text="en attente">
       <formula>NOT(ISERROR(SEARCH("en attente",D38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="Corrigé">
+    <cfRule type="containsText" dxfId="28" priority="40" operator="containsText" text="Corrigé">
       <formula>NOT(ISERROR(SEARCH("Corrigé",D38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Abandonné">
+    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="Abandonné">
       <formula>NOT(ISERROR(SEARCH("Abandonné",D42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="en attente">
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="en attente">
       <formula>NOT(ISERROR(SEARCH("en attente",D42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="Corrigé">
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="Corrigé">
       <formula>NOT(ISERROR(SEARCH("Corrigé",D42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Abandonné">
+    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="Abandonné">
       <formula>NOT(ISERROR(SEARCH("Abandonné",D41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="en attente">
+    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="en attente">
       <formula>NOT(ISERROR(SEARCH("en attente",D41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="Corrigé">
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="Corrigé">
       <formula>NOT(ISERROR(SEARCH("Corrigé",D41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Abandonné">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Abandonné">
       <formula>NOT(ISERROR(SEARCH("Abandonné",D40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="en attente">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="en attente">
       <formula>NOT(ISERROR(SEARCH("en attente",D40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Corrigé">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Corrigé">
       <formula>NOT(ISERROR(SEARCH("Corrigé",D40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Abandonné">
+      <formula>NOT(ISERROR(SEARCH("Abandonné",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="en attente">
+      <formula>NOT(ISERROR(SEARCH("en attente",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="Corrigé">
+      <formula>NOT(ISERROR(SEARCH("Corrigé",D39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Abandonné">
+      <formula>NOT(ISERROR(SEARCH("Abandonné",D58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="en attente">
+      <formula>NOT(ISERROR(SEARCH("en attente",D58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="Corrigé">
+      <formula>NOT(ISERROR(SEARCH("Corrigé",D58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Abandonné">
+      <formula>NOT(ISERROR(SEARCH("Abandonné",D55)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D55)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="en attente">
+      <formula>NOT(ISERROR(SEARCH("en attente",D55)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Corrigé">
+      <formula>NOT(ISERROR(SEARCH("Corrigé",D55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Abandonné">
-      <formula>NOT(ISERROR(SEARCH("Abandonné",D39)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Abandonné",D56)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D39)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D56)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="en attente">
-      <formula>NOT(ISERROR(SEARCH("en attente",D39)))</formula>
+      <formula>NOT(ISERROR(SEARCH("en attente",D56)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Corrigé">
-      <formula>NOT(ISERROR(SEARCH("Corrigé",D39)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Corrigé",D56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mise à jour liste de tests et manuel d'utilisation + modification historique absences
</commit_message>
<xml_diff>
--- a/Liste_des_tests.xlsx
+++ b/Liste_des_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="121">
   <si>
     <t>Trombinoscope</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>Absences/Retards</t>
-  </si>
-  <si>
-    <t>Ajout d'un retard</t>
   </si>
   <si>
     <t>bug détecté : on ne sait pas si l'ajout a été effectué</t>
@@ -368,6 +365,21 @@
   </si>
   <si>
     <t>bug détecté : le format de l'heure dans la date n'est pas bon : l'heure est 00:00:00. Voir fomat de date à l'affichage</t>
+  </si>
+  <si>
+    <t>Ajout d'un retard du matin</t>
+  </si>
+  <si>
+    <t>Ajout d'un retard du midi</t>
+  </si>
+  <si>
+    <t>bug déteccté : impossible, le champs est grisé</t>
+  </si>
+  <si>
+    <t>Clic sur le bouton Annuler puis sur Enregistrer</t>
+  </si>
+  <si>
+    <t>bug détecté : exception non gérée lors de la vérification de saisie (sur les dates)</t>
   </si>
 </sst>
 </file>
@@ -437,94 +449,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -1112,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76:D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,13 +1094,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1212,7 +1137,7 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>13</v>
@@ -1220,10 +1145,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
         <v>78</v>
-      </c>
-      <c r="C13" t="s">
-        <v>79</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>13</v>
@@ -1247,7 +1172,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>13</v>
@@ -1313,10 +1238,10 @@
     </row>
     <row r="25" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>13</v>
@@ -1324,15 +1249,15 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" t="s">
         <v>93</v>
-      </c>
-      <c r="C27" t="s">
-        <v>94</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>13</v>
@@ -1340,77 +1265,77 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1428,10 +1353,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" t="s">
         <v>115</v>
-      </c>
-      <c r="C46" t="s">
-        <v>116</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>13</v>
@@ -1453,7 +1378,7 @@
         <v>33</v>
       </c>
       <c r="C48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>13</v>
@@ -1493,12 +1418,12 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1508,17 +1433,17 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1531,10 +1456,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" t="s">
         <v>43</v>
-      </c>
-      <c r="C60" t="s">
-        <v>44</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>13</v>
@@ -1542,10 +1467,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="C61" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>13</v>
@@ -1553,10 +1478,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C62" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>13</v>
@@ -1564,34 +1489,34 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C63" t="s">
-        <v>83</v>
+        <v>47</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="C64" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>51</v>
-      </c>
-      <c r="C65" t="s">
-        <v>52</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C66" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>13</v>
@@ -1599,10 +1524,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C67" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>13</v>
@@ -1610,31 +1535,31 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>55</v>
+        <v>46</v>
+      </c>
+      <c r="C68" t="s">
+        <v>75</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>57</v>
-      </c>
-      <c r="C70" t="s">
-        <v>52</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C71" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>13</v>
@@ -1642,10 +1567,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>13</v>
@@ -1653,50 +1578,67 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
+        <v>58</v>
+      </c>
+      <c r="C73" t="s">
+        <v>59</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>119</v>
+      </c>
+      <c r="C75" t="s">
+        <v>120</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>63</v>
-      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1705,71 +1647,76 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
+      <c r="B84" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>84</v>
       </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
+      <c r="C86" t="s">
         <v>85</v>
       </c>
-      <c r="C85" t="s">
-        <v>86</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
+      <c r="D86" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>70</v>
-      </c>
-      <c r="C87" t="s">
-        <v>71</v>
-      </c>
+      <c r="A87" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="C88" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>73</v>
-      </c>
-      <c r="C89" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C90" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>73</v>
+      </c>
+      <c r="C91" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A87:D87"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A44:D44"/>
     <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A85:D85"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D26 D44:D54 D59:D1048576 D57">
     <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="Abandonné">

</xml_diff>

<commit_message>
Mise à jour des docs
</commit_message>
<xml_diff>
--- a/Liste_des_tests.xlsx
+++ b/Liste_des_tests.xlsx
@@ -79,9 +79,6 @@
     <t>Affichage des information du contact du stagiaire</t>
   </si>
   <si>
-    <t>bug détecté : s'il y a plusieurs contacts ? ET d’où sort le "TUT" ? -&gt; pas dans l'appli administrative</t>
-  </si>
-  <si>
     <t>Affichage des différents seuils d'absences</t>
   </si>
   <si>
@@ -269,9 +266,6 @@
   </si>
   <si>
     <t>bug détecté : Lors de la modification d'un contact, on peut lui enlever ses 2 numéros de téléphone</t>
-  </si>
-  <si>
-    <t>bug détecté : le contact et le stagiaire sont liés bizarrement, ça ne tient pas trop la route. La correction apporte une gestion plus souple.</t>
   </si>
   <si>
     <t>Ajout d'un contact provenant d'une entreprise existante</t>
@@ -378,6 +372,12 @@
   </si>
   <si>
     <t>bug détecté : exception non gérée</t>
+  </si>
+  <si>
+    <t>bug détecté : Revoir les liens entre contacts et stagiaires. La correction apporte une gestion plus souple.</t>
+  </si>
+  <si>
+    <t>bug détecté : impossible de gérer de multiples contacts</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -507,6 +506,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -514,18 +526,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,11 +862,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="189014784"/>
-        <c:axId val="189028608"/>
+        <c:axId val="174488192"/>
+        <c:axId val="174514560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="189014784"/>
+        <c:axId val="174488192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -875,7 +875,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189028608"/>
+        <c:crossAx val="174514560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -883,7 +883,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189028608"/>
+        <c:axId val="174514560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -893,14 +893,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189014784"/>
+        <c:crossAx val="174488192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1240,8 +1239,8 @@
   </sheetPr>
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,832 +1265,832 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D17" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="9"/>
+      <c r="B44" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="7"/>
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="10"/>
+      <c r="B54" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="7"/>
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="B55" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="7"/>
+      <c r="D55" s="8"/>
+    </row>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" s="7"/>
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="B57" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" s="7"/>
+      <c r="D57" s="8"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="9"/>
+      <c r="B59" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="10"/>
+      <c r="B60" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="10"/>
+      <c r="B61" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="10"/>
+      <c r="B62" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="10"/>
+      <c r="B63" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D63" s="8"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="10"/>
+      <c r="B64" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64" s="7"/>
+      <c r="D64" s="8"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="10"/>
+      <c r="B65" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="10"/>
+      <c r="B66" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="10"/>
+      <c r="B67" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="10"/>
+      <c r="B68" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C68" s="7"/>
+      <c r="D68" s="8"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="10"/>
+      <c r="B69" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C69" s="7"/>
+      <c r="D69" s="8"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="10"/>
+      <c r="B70" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="10"/>
+      <c r="B71" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="10"/>
+      <c r="B72" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="10"/>
+      <c r="B73" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C73" s="7"/>
+      <c r="D73" s="8"/>
+    </row>
+    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="11"/>
+      <c r="B74" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="9"/>
+      <c r="B76" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76" s="7"/>
+      <c r="D76" s="8"/>
+    </row>
+    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="10"/>
+      <c r="B77" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77" s="7"/>
+      <c r="D77" s="8"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="10"/>
+      <c r="B78" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C78" s="7"/>
+      <c r="D78" s="8"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="10"/>
+      <c r="B79" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C79" s="7"/>
+      <c r="D79" s="8"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="10"/>
+      <c r="B80" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C80" s="7"/>
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="10"/>
+      <c r="B81" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C81" s="7"/>
+      <c r="D81" s="8"/>
+    </row>
+    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="10"/>
+      <c r="B82" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C82" s="7"/>
+      <c r="D82" s="8"/>
+    </row>
+    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="11"/>
+      <c r="B83" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C83" s="7"/>
+      <c r="D83" s="8"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B84" s="12"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+    </row>
+    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="6"/>
+      <c r="B85" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B86" s="12"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="9"/>
+      <c r="B87" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D87" s="8"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="10"/>
+      <c r="B88" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C88" s="7"/>
+      <c r="D88" s="8"/>
+    </row>
+    <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="10"/>
+      <c r="B89" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D89" s="8"/>
+    </row>
+    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="11"/>
+      <c r="B90" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-    </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-    </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="9"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-    </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-      <c r="B46" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="B47" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="9"/>
-    </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
-      <c r="B49" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
-      <c r="B50" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
-    </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="B51" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
-      <c r="B52" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
-      <c r="B53" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C53" s="8"/>
-      <c r="D53" s="9"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
-      <c r="B54" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="9"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
-      <c r="B55" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
-    </row>
-    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
-      <c r="B56" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="9"/>
-    </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
-      <c r="B60" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
-      <c r="B61" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
-      <c r="B62" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
-      <c r="B63" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D63" s="9"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
-      <c r="B64" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="9"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
-      <c r="B65" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
-      <c r="B67" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
-      <c r="B68" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C68" s="8"/>
-      <c r="D68" s="9"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
-      <c r="B69" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="9"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="B70" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
-      <c r="B71" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
-      <c r="B72" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
-      <c r="B73" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C73" s="8"/>
-      <c r="D73" s="9"/>
-    </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="16"/>
-      <c r="B74" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D74" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
-      <c r="B76" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C76" s="8"/>
-      <c r="D76" s="9"/>
-    </row>
-    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-      <c r="B77" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C77" s="8"/>
-      <c r="D77" s="9"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
-      <c r="B78" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C78" s="8"/>
-      <c r="D78" s="9"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
-      <c r="B79" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C79" s="8"/>
-      <c r="D79" s="9"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="15"/>
-      <c r="B80" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C80" s="8"/>
-      <c r="D80" s="9"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="15"/>
-      <c r="B81" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C81" s="8"/>
-      <c r="D81" s="9"/>
-    </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="15"/>
-      <c r="B82" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C82" s="8"/>
-      <c r="D82" s="9"/>
-    </row>
-    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="16"/>
-      <c r="B83" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C83" s="8"/>
-      <c r="D83" s="9"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
-    </row>
-    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="7"/>
-      <c r="B85" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D85" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B86" s="13"/>
-      <c r="C86" s="13"/>
-      <c r="D86" s="13"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
-      <c r="B87" s="8" t="s">
+      <c r="C90" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C87" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D87" s="9"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="15"/>
-      <c r="B88" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C88" s="8"/>
-      <c r="D88" s="9"/>
-    </row>
-    <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="15"/>
-      <c r="B89" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D89" s="9"/>
-    </row>
-    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="16"/>
-      <c r="B90" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D90" s="9"/>
+      <c r="D90" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>